<commit_message>
Fin de exercice 1.1 Notes
</commit_message>
<xml_diff>
--- a/TP1/data/sy02-p2016.xlsx
+++ b/TP1/data/sy02-p2016.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="sy02_p2016" localSheetId="0">Feuil1!$A$1:$K$297</definedName>
-  </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -24,28 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="sy02-p2016" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/raphael/Documents/Etudes_Informatique/Cours/UTC/GI04/SY09_Data_Mining/UTC_SY09_TPs/TP1/data/sy02-p2016.csv" decimal="," thousands=" " comma="1">
-      <textFields count="11">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1530,8 +1505,30 @@
 </styleSheet>
 </file>
 
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="sy02-p2016" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:K297" totalsRowShown="0">
+  <autoFilter ref="A1:K297">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="TC"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="11">
+    <tableColumn id="1" name="nom"/>
+    <tableColumn id="2" name="specialite"/>
+    <tableColumn id="3" name="niveau"/>
+    <tableColumn id="4" name="statut"/>
+    <tableColumn id="5" name="dernier diplome obtenu"/>
+    <tableColumn id="6" name="note median"/>
+    <tableColumn id="7" name="correcteur median"/>
+    <tableColumn id="8" name="note final"/>
+    <tableColumn id="9" name="correcteur final"/>
+    <tableColumn id="10" name="note totale"/>
+    <tableColumn id="11" name="resultat"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1799,21 +1796,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K297"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K306" sqref="K306"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -1851,7 +1850,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1886,7 +1885,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1921,7 +1920,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1956,7 +1955,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1991,7 +1990,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -2026,7 +2025,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2061,7 +2060,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -2096,7 +2095,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -2131,7 +2130,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -2166,7 +2165,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -2201,7 +2200,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -2236,7 +2235,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -2271,7 +2270,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -2341,7 +2340,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -2367,7 +2366,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>78</v>
       </c>
@@ -2402,7 +2401,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -2437,7 +2436,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -2472,7 +2471,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -2507,7 +2506,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>90</v>
       </c>
@@ -2577,7 +2576,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -2612,7 +2611,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -2647,7 +2646,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -2682,7 +2681,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -2717,7 +2716,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>101</v>
       </c>
@@ -2752,7 +2751,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -2784,7 +2783,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -2819,7 +2818,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -2854,7 +2853,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -2889,7 +2888,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>116</v>
       </c>
@@ -2924,7 +2923,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>117</v>
       </c>
@@ -2959,7 +2958,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>118</v>
       </c>
@@ -2994,7 +2993,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>120</v>
       </c>
@@ -3029,7 +3028,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>121</v>
       </c>
@@ -3064,7 +3063,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>123</v>
       </c>
@@ -3099,7 +3098,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>125</v>
       </c>
@@ -3134,7 +3133,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>129</v>
       </c>
@@ -3169,7 +3168,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>131</v>
       </c>
@@ -3204,7 +3203,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>132</v>
       </c>
@@ -3230,7 +3229,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>133</v>
       </c>
@@ -3256,7 +3255,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>134</v>
       </c>
@@ -3291,7 +3290,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>136</v>
       </c>
@@ -3326,7 +3325,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>138</v>
       </c>
@@ -3361,7 +3360,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>140</v>
       </c>
@@ -3396,7 +3395,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>142</v>
       </c>
@@ -3431,7 +3430,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>143</v>
       </c>
@@ -3466,7 +3465,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>144</v>
       </c>
@@ -3501,7 +3500,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>145</v>
       </c>
@@ -3536,7 +3535,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>147</v>
       </c>
@@ -3571,7 +3570,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>148</v>
       </c>
@@ -3606,7 +3605,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>150</v>
       </c>
@@ -3641,7 +3640,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>153</v>
       </c>
@@ -3676,7 +3675,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>156</v>
       </c>
@@ -3711,7 +3710,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>158</v>
       </c>
@@ -3746,7 +3745,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>160</v>
       </c>
@@ -3781,7 +3780,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -3816,7 +3815,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>164</v>
       </c>
@@ -3851,7 +3850,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -3886,7 +3885,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>168</v>
       </c>
@@ -3921,7 +3920,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>171</v>
       </c>
@@ -3956,7 +3955,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>172</v>
       </c>
@@ -3991,7 +3990,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>173</v>
       </c>
@@ -4026,7 +4025,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>176</v>
       </c>
@@ -4061,7 +4060,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>178</v>
       </c>
@@ -4087,7 +4086,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>179</v>
       </c>
@@ -4122,7 +4121,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>181</v>
       </c>
@@ -4157,7 +4156,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>182</v>
       </c>
@@ -4192,7 +4191,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>183</v>
       </c>
@@ -4227,7 +4226,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>185</v>
       </c>
@@ -4262,7 +4261,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>187</v>
       </c>
@@ -4297,7 +4296,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>188</v>
       </c>
@@ -4332,7 +4331,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>190</v>
       </c>
@@ -4367,7 +4366,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>192</v>
       </c>
@@ -4402,7 +4401,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>193</v>
       </c>
@@ -4428,7 +4427,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>194</v>
       </c>
@@ -4463,7 +4462,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -4495,7 +4494,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>197</v>
       </c>
@@ -4530,7 +4529,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>199</v>
       </c>
@@ -4565,7 +4564,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>200</v>
       </c>
@@ -4600,7 +4599,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>202</v>
       </c>
@@ -4635,7 +4634,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>204</v>
       </c>
@@ -4670,7 +4669,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>206</v>
       </c>
@@ -4705,7 +4704,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>208</v>
       </c>
@@ -4725,7 +4724,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>209</v>
       </c>
@@ -4760,7 +4759,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>210</v>
       </c>
@@ -4795,7 +4794,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>211</v>
       </c>
@@ -4830,7 +4829,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>212</v>
       </c>
@@ -4865,7 +4864,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>214</v>
       </c>
@@ -4900,7 +4899,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>216</v>
       </c>
@@ -4935,7 +4934,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>218</v>
       </c>
@@ -4970,7 +4969,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>220</v>
       </c>
@@ -5005,7 +5004,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>221</v>
       </c>
@@ -5040,7 +5039,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>222</v>
       </c>
@@ -5075,7 +5074,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>224</v>
       </c>
@@ -5110,7 +5109,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>225</v>
       </c>
@@ -5145,7 +5144,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>226</v>
       </c>
@@ -5180,7 +5179,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>227</v>
       </c>
@@ -5215,7 +5214,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>228</v>
       </c>
@@ -5285,7 +5284,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>231</v>
       </c>
@@ -5320,7 +5319,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>232</v>
       </c>
@@ -5355,7 +5354,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>233</v>
       </c>
@@ -5390,7 +5389,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>234</v>
       </c>
@@ -5425,7 +5424,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>236</v>
       </c>
@@ -5460,7 +5459,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>238</v>
       </c>
@@ -5495,7 +5494,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>239</v>
       </c>
@@ -5530,7 +5529,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>240</v>
       </c>
@@ -5565,7 +5564,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>241</v>
       </c>
@@ -5600,7 +5599,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>243</v>
       </c>
@@ -5635,7 +5634,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>244</v>
       </c>
@@ -5670,7 +5669,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>245</v>
       </c>
@@ -5705,7 +5704,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>247</v>
       </c>
@@ -5740,7 +5739,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>249</v>
       </c>
@@ -5775,7 +5774,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>250</v>
       </c>
@@ -5810,7 +5809,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>252</v>
       </c>
@@ -5845,7 +5844,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>253</v>
       </c>
@@ -5880,7 +5879,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>254</v>
       </c>
@@ -5915,7 +5914,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>256</v>
       </c>
@@ -5950,7 +5949,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>257</v>
       </c>
@@ -5985,7 +5984,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>259</v>
       </c>
@@ -6020,7 +6019,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>261</v>
       </c>
@@ -6055,7 +6054,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>263</v>
       </c>
@@ -6116,7 +6115,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>266</v>
       </c>
@@ -6151,7 +6150,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>268</v>
       </c>
@@ -6186,7 +6185,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>269</v>
       </c>
@@ -6221,7 +6220,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>270</v>
       </c>
@@ -6276,7 +6275,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>272</v>
       </c>
@@ -6311,7 +6310,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>273</v>
       </c>
@@ -6346,7 +6345,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>274</v>
       </c>
@@ -6381,7 +6380,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>275</v>
       </c>
@@ -6416,7 +6415,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>276</v>
       </c>
@@ -6451,7 +6450,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>277</v>
       </c>
@@ -6486,7 +6485,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>278</v>
       </c>
@@ -6521,7 +6520,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>280</v>
       </c>
@@ -6556,7 +6555,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>282</v>
       </c>
@@ -6591,7 +6590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>284</v>
       </c>
@@ -6626,7 +6625,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>285</v>
       </c>
@@ -6661,7 +6660,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>286</v>
       </c>
@@ -6696,7 +6695,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>287</v>
       </c>
@@ -6731,7 +6730,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>289</v>
       </c>
@@ -6766,7 +6765,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>290</v>
       </c>
@@ -6801,7 +6800,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>291</v>
       </c>
@@ -6836,7 +6835,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>292</v>
       </c>
@@ -6853,7 +6852,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>293</v>
       </c>
@@ -6888,7 +6887,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>295</v>
       </c>
@@ -6923,7 +6922,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>296</v>
       </c>
@@ -6958,7 +6957,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>297</v>
       </c>
@@ -6993,7 +6992,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>298</v>
       </c>
@@ -7028,7 +7027,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>299</v>
       </c>
@@ -7063,7 +7062,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>300</v>
       </c>
@@ -7133,7 +7132,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>302</v>
       </c>
@@ -7159,7 +7158,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>303</v>
       </c>
@@ -7194,7 +7193,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>304</v>
       </c>
@@ -7229,7 +7228,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>305</v>
       </c>
@@ -7264,7 +7263,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>306</v>
       </c>
@@ -7299,7 +7298,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>307</v>
       </c>
@@ -7334,7 +7333,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>308</v>
       </c>
@@ -7369,7 +7368,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>313</v>
       </c>
@@ -7404,7 +7403,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>314</v>
       </c>
@@ -7439,7 +7438,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>316</v>
       </c>
@@ -7474,7 +7473,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>317</v>
       </c>
@@ -7509,7 +7508,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>318</v>
       </c>
@@ -7544,7 +7543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>319</v>
       </c>
@@ -7614,7 +7613,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>321</v>
       </c>
@@ -7649,7 +7648,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>322</v>
       </c>
@@ -7675,7 +7674,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>323</v>
       </c>
@@ -7710,7 +7709,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>325</v>
       </c>
@@ -7742,7 +7741,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>326</v>
       </c>
@@ -7777,7 +7776,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>327</v>
       </c>
@@ -7847,7 +7846,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>329</v>
       </c>
@@ -7882,7 +7881,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>330</v>
       </c>
@@ -7917,7 +7916,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>331</v>
       </c>
@@ -7952,7 +7951,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>332</v>
       </c>
@@ -7987,7 +7986,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>333</v>
       </c>
@@ -8022,7 +8021,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>335</v>
       </c>
@@ -8057,7 +8056,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>337</v>
       </c>
@@ -8127,7 +8126,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>339</v>
       </c>
@@ -8162,7 +8161,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>340</v>
       </c>
@@ -8194,7 +8193,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>343</v>
       </c>
@@ -8229,7 +8228,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>345</v>
       </c>
@@ -8264,7 +8263,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>346</v>
       </c>
@@ -8299,7 +8298,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>348</v>
       </c>
@@ -8334,7 +8333,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>349</v>
       </c>
@@ -8369,7 +8368,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>350</v>
       </c>
@@ -8404,7 +8403,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>351</v>
       </c>
@@ -8439,7 +8438,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>352</v>
       </c>
@@ -8474,7 +8473,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>353</v>
       </c>
@@ -8544,7 +8543,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>355</v>
       </c>
@@ -8570,7 +8569,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>356</v>
       </c>
@@ -8605,7 +8604,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>357</v>
       </c>
@@ -8640,7 +8639,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>358</v>
       </c>
@@ -8675,7 +8674,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>359</v>
       </c>
@@ -8710,7 +8709,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>360</v>
       </c>
@@ -8745,7 +8744,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>361</v>
       </c>
@@ -8780,7 +8779,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>362</v>
       </c>
@@ -8815,7 +8814,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>364</v>
       </c>
@@ -8850,7 +8849,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>365</v>
       </c>
@@ -8885,7 +8884,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>366</v>
       </c>
@@ -8920,7 +8919,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>367</v>
       </c>
@@ -8955,7 +8954,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>368</v>
       </c>
@@ -8990,7 +8989,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>370</v>
       </c>
@@ -9025,7 +9024,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>371</v>
       </c>
@@ -9060,7 +9059,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>372</v>
       </c>
@@ -9095,7 +9094,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>373</v>
       </c>
@@ -9130,7 +9129,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>375</v>
       </c>
@@ -9165,7 +9164,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>376</v>
       </c>
@@ -9200,7 +9199,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>377</v>
       </c>
@@ -9235,7 +9234,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>378</v>
       </c>
@@ -9270,7 +9269,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>379</v>
       </c>
@@ -9305,7 +9304,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>380</v>
       </c>
@@ -9340,7 +9339,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>381</v>
       </c>
@@ -9375,7 +9374,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>382</v>
       </c>
@@ -9410,7 +9409,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>383</v>
       </c>
@@ -9445,7 +9444,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>384</v>
       </c>
@@ -9515,7 +9514,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>386</v>
       </c>
@@ -9550,7 +9549,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>387</v>
       </c>
@@ -9585,7 +9584,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>388</v>
       </c>
@@ -9620,7 +9619,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>389</v>
       </c>
@@ -9655,7 +9654,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>390</v>
       </c>
@@ -9690,7 +9689,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>391</v>
       </c>
@@ -9725,7 +9724,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>393</v>
       </c>
@@ -9760,7 +9759,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>394</v>
       </c>
@@ -9795,7 +9794,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>395</v>
       </c>
@@ -9830,7 +9829,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>396</v>
       </c>
@@ -9865,7 +9864,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>398</v>
       </c>
@@ -9900,7 +9899,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>399</v>
       </c>
@@ -9935,7 +9934,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>401</v>
       </c>
@@ -9970,7 +9969,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>402</v>
       </c>
@@ -10005,7 +10004,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>403</v>
       </c>
@@ -10040,7 +10039,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>404</v>
       </c>
@@ -10075,7 +10074,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>406</v>
       </c>
@@ -10110,7 +10109,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>407</v>
       </c>
@@ -10145,7 +10144,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>409</v>
       </c>
@@ -10180,7 +10179,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>410</v>
       </c>
@@ -10215,7 +10214,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>411</v>
       </c>
@@ -10250,7 +10249,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>412</v>
       </c>
@@ -10285,7 +10284,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>414</v>
       </c>
@@ -10320,7 +10319,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>415</v>
       </c>
@@ -10355,7 +10354,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>416</v>
       </c>
@@ -10390,7 +10389,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>417</v>
       </c>
@@ -10425,7 +10424,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>419</v>
       </c>
@@ -10460,7 +10459,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>420</v>
       </c>
@@ -10495,7 +10494,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>421</v>
       </c>
@@ -10530,7 +10529,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>422</v>
       </c>
@@ -10562,7 +10561,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>424</v>
       </c>
@@ -10597,7 +10596,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>425</v>
       </c>
@@ -10632,7 +10631,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>426</v>
       </c>
@@ -10667,7 +10666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>427</v>
       </c>
@@ -10702,7 +10701,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>429</v>
       </c>
@@ -10737,7 +10736,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>430</v>
       </c>
@@ -10772,7 +10771,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>431</v>
       </c>
@@ -10807,7 +10806,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>432</v>
       </c>
@@ -10842,7 +10841,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>434</v>
       </c>
@@ -10877,7 +10876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>435</v>
       </c>
@@ -10912,7 +10911,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>436</v>
       </c>
@@ -10947,7 +10946,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>437</v>
       </c>
@@ -10982,7 +10981,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>439</v>
       </c>
@@ -11017,7 +11016,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>440</v>
       </c>
@@ -11052,7 +11051,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>441</v>
       </c>
@@ -11087,7 +11086,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>442</v>
       </c>
@@ -11122,7 +11121,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>444</v>
       </c>
@@ -11157,7 +11156,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>445</v>
       </c>
@@ -11192,7 +11191,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>446</v>
       </c>
@@ -11227,7 +11226,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>448</v>
       </c>
@@ -11262,7 +11261,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>449</v>
       </c>
@@ -11297,7 +11296,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>450</v>
       </c>
@@ -11332,7 +11331,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>451</v>
       </c>
@@ -11367,7 +11366,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>452</v>
       </c>
@@ -11402,7 +11401,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>453</v>
       </c>
@@ -11437,7 +11436,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>454</v>
       </c>
@@ -11507,7 +11506,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>457</v>
       </c>
@@ -11542,7 +11541,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>459</v>
       </c>
@@ -11577,7 +11576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>460</v>
       </c>
@@ -11612,7 +11611,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>461</v>
       </c>
@@ -11647,7 +11646,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>462</v>
       </c>
@@ -11682,7 +11681,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>463</v>
       </c>
@@ -11717,7 +11716,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>465</v>
       </c>
@@ -11752,7 +11751,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>466</v>
       </c>
@@ -11787,7 +11786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>468</v>
       </c>
@@ -11822,7 +11821,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>469</v>
       </c>
@@ -11857,7 +11856,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>470</v>
       </c>
@@ -11892,7 +11891,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>471</v>
       </c>
@@ -11927,7 +11926,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>472</v>
       </c>
@@ -11962,7 +11961,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>474</v>
       </c>
@@ -11997,7 +11996,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>475</v>
       </c>
@@ -12032,7 +12031,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>476</v>
       </c>
@@ -12069,5 +12068,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Pas important : changement de filtre dans une colonne de sy02-p2016.xlsx
</commit_message>
<xml_diff>
--- a/TP1/data/sy02-p2016.xlsx
+++ b/TP1/data/sy02-p2016.xlsx
@@ -1461,8 +1461,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1489,8 +1496,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1507,13 +1515,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:K297" totalsRowShown="0">
-  <autoFilter ref="A1:K297">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="TC"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K297"/>
   <tableColumns count="11">
     <tableColumn id="1" name="nom"/>
     <tableColumn id="2" name="specialite"/>
@@ -1797,7 +1799,7 @@
   <dimension ref="A1:K297"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K306" sqref="K306"/>
+      <selection activeCell="G147" sqref="G147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1850,7 +1852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1885,7 +1887,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1920,7 +1922,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1955,7 +1957,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1990,7 +1992,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -2025,7 +2027,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2060,7 +2062,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -2095,7 +2097,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -2130,7 +2132,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -2165,7 +2167,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -2200,7 +2202,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -2235,7 +2237,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -2270,7 +2272,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -2340,7 +2342,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -2366,7 +2368,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>78</v>
       </c>
@@ -2401,7 +2403,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -2436,7 +2438,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>84</v>
       </c>
@@ -2471,7 +2473,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>86</v>
       </c>
@@ -2506,7 +2508,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -2541,7 +2543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>90</v>
       </c>
@@ -2576,7 +2578,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -2611,7 +2613,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -2646,7 +2648,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -2681,7 +2683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -2716,7 +2718,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>101</v>
       </c>
@@ -2751,7 +2753,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -2783,7 +2785,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -2818,7 +2820,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -2853,7 +2855,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -2888,7 +2890,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>116</v>
       </c>
@@ -2923,7 +2925,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>117</v>
       </c>
@@ -2958,7 +2960,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>118</v>
       </c>
@@ -2993,7 +2995,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>120</v>
       </c>
@@ -3028,7 +3030,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>121</v>
       </c>
@@ -3063,7 +3065,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>123</v>
       </c>
@@ -3098,7 +3100,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>125</v>
       </c>
@@ -3133,7 +3135,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>129</v>
       </c>
@@ -3168,7 +3170,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>131</v>
       </c>
@@ -3203,7 +3205,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>132</v>
       </c>
@@ -3229,7 +3231,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>133</v>
       </c>
@@ -3255,7 +3257,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>134</v>
       </c>
@@ -3290,7 +3292,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>136</v>
       </c>
@@ -3325,7 +3327,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>138</v>
       </c>
@@ -3360,7 +3362,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>140</v>
       </c>
@@ -3395,7 +3397,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>142</v>
       </c>
@@ -3430,7 +3432,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>143</v>
       </c>
@@ -3465,7 +3467,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>144</v>
       </c>
@@ -3500,7 +3502,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>145</v>
       </c>
@@ -3535,7 +3537,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>147</v>
       </c>
@@ -3570,7 +3572,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>148</v>
       </c>
@@ -3605,7 +3607,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>150</v>
       </c>
@@ -3640,7 +3642,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>153</v>
       </c>
@@ -3675,7 +3677,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>156</v>
       </c>
@@ -3710,7 +3712,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>158</v>
       </c>
@@ -3745,7 +3747,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>160</v>
       </c>
@@ -3780,7 +3782,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>163</v>
       </c>
@@ -3815,7 +3817,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>164</v>
       </c>
@@ -3850,7 +3852,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>166</v>
       </c>
@@ -3885,7 +3887,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>168</v>
       </c>
@@ -3920,7 +3922,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>171</v>
       </c>
@@ -3955,7 +3957,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>172</v>
       </c>
@@ -3990,7 +3992,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>173</v>
       </c>
@@ -4025,7 +4027,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>176</v>
       </c>
@@ -4060,7 +4062,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>178</v>
       </c>
@@ -4086,7 +4088,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>179</v>
       </c>
@@ -4121,7 +4123,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>181</v>
       </c>
@@ -4156,7 +4158,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>182</v>
       </c>
@@ -4191,7 +4193,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>183</v>
       </c>
@@ -4226,7 +4228,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>185</v>
       </c>
@@ -4261,7 +4263,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>187</v>
       </c>
@@ -4296,7 +4298,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>188</v>
       </c>
@@ -4331,7 +4333,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>190</v>
       </c>
@@ -4366,7 +4368,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>192</v>
       </c>
@@ -4401,7 +4403,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>193</v>
       </c>
@@ -4427,7 +4429,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>194</v>
       </c>
@@ -4462,7 +4464,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>196</v>
       </c>
@@ -4494,7 +4496,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>197</v>
       </c>
@@ -4529,7 +4531,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>199</v>
       </c>
@@ -4564,7 +4566,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>200</v>
       </c>
@@ -4599,7 +4601,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>202</v>
       </c>
@@ -4634,7 +4636,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>204</v>
       </c>
@@ -4669,7 +4671,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>206</v>
       </c>
@@ -4704,7 +4706,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>208</v>
       </c>
@@ -4724,7 +4726,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>209</v>
       </c>
@@ -4759,7 +4761,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>210</v>
       </c>
@@ -4794,7 +4796,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>211</v>
       </c>
@@ -4829,7 +4831,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>212</v>
       </c>
@@ -4864,7 +4866,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>214</v>
       </c>
@@ -4899,7 +4901,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>216</v>
       </c>
@@ -4934,7 +4936,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>218</v>
       </c>
@@ -4969,7 +4971,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>220</v>
       </c>
@@ -5004,7 +5006,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>221</v>
       </c>
@@ -5039,7 +5041,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>222</v>
       </c>
@@ -5074,7 +5076,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>224</v>
       </c>
@@ -5109,7 +5111,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>225</v>
       </c>
@@ -5144,7 +5146,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>226</v>
       </c>
@@ -5179,7 +5181,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>227</v>
       </c>
@@ -5214,7 +5216,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>228</v>
       </c>
@@ -5284,7 +5286,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>231</v>
       </c>
@@ -5319,7 +5321,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>232</v>
       </c>
@@ -5354,7 +5356,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>233</v>
       </c>
@@ -5389,7 +5391,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>234</v>
       </c>
@@ -5424,7 +5426,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>236</v>
       </c>
@@ -5459,7 +5461,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>238</v>
       </c>
@@ -5494,7 +5496,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>239</v>
       </c>
@@ -5529,7 +5531,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>240</v>
       </c>
@@ -5564,7 +5566,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>241</v>
       </c>
@@ -5599,7 +5601,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>243</v>
       </c>
@@ -5634,7 +5636,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>244</v>
       </c>
@@ -5669,7 +5671,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>245</v>
       </c>
@@ -5704,7 +5706,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>247</v>
       </c>
@@ -5739,7 +5741,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>249</v>
       </c>
@@ -5774,7 +5776,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>250</v>
       </c>
@@ -5809,7 +5811,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>252</v>
       </c>
@@ -5844,7 +5846,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>253</v>
       </c>
@@ -5879,7 +5881,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>254</v>
       </c>
@@ -5914,7 +5916,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>256</v>
       </c>
@@ -5949,7 +5951,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>257</v>
       </c>
@@ -5984,7 +5986,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>259</v>
       </c>
@@ -6019,7 +6021,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>261</v>
       </c>
@@ -6054,7 +6056,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>263</v>
       </c>
@@ -6115,7 +6117,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>266</v>
       </c>
@@ -6150,7 +6152,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>268</v>
       </c>
@@ -6185,7 +6187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>269</v>
       </c>
@@ -6220,7 +6222,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>270</v>
       </c>
@@ -6275,7 +6277,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>272</v>
       </c>
@@ -6310,7 +6312,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>273</v>
       </c>
@@ -6345,7 +6347,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>274</v>
       </c>
@@ -6380,7 +6382,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>275</v>
       </c>
@@ -6415,7 +6417,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>276</v>
       </c>
@@ -6450,7 +6452,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>277</v>
       </c>
@@ -6485,7 +6487,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>278</v>
       </c>
@@ -6520,7 +6522,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>280</v>
       </c>
@@ -6555,7 +6557,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>282</v>
       </c>
@@ -6590,7 +6592,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>284</v>
       </c>
@@ -6625,7 +6627,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>285</v>
       </c>
@@ -6660,7 +6662,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>286</v>
       </c>
@@ -6695,7 +6697,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>287</v>
       </c>
@@ -6730,7 +6732,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>289</v>
       </c>
@@ -6765,7 +6767,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>290</v>
       </c>
@@ -6800,7 +6802,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>291</v>
       </c>
@@ -6835,7 +6837,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>292</v>
       </c>
@@ -6848,11 +6850,12 @@
       <c r="D147" t="s">
         <v>104</v>
       </c>
+      <c r="G147" s="1"/>
       <c r="K147" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>293</v>
       </c>
@@ -6887,7 +6890,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>295</v>
       </c>
@@ -6922,7 +6925,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>296</v>
       </c>
@@ -6957,7 +6960,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>297</v>
       </c>
@@ -6992,7 +6995,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>298</v>
       </c>
@@ -7027,7 +7030,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>299</v>
       </c>
@@ -7062,7 +7065,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>300</v>
       </c>
@@ -7132,7 +7135,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>302</v>
       </c>
@@ -7158,7 +7161,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>303</v>
       </c>
@@ -7193,7 +7196,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>304</v>
       </c>
@@ -7228,7 +7231,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>305</v>
       </c>
@@ -7263,7 +7266,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>306</v>
       </c>
@@ -7298,7 +7301,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>307</v>
       </c>
@@ -7333,7 +7336,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>308</v>
       </c>
@@ -7368,7 +7371,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>313</v>
       </c>
@@ -7403,7 +7406,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>314</v>
       </c>
@@ -7438,7 +7441,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>316</v>
       </c>
@@ -7473,7 +7476,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>317</v>
       </c>
@@ -7508,7 +7511,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>318</v>
       </c>
@@ -7543,7 +7546,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>319</v>
       </c>
@@ -7613,7 +7616,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>321</v>
       </c>
@@ -7648,7 +7651,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>322</v>
       </c>
@@ -7674,7 +7677,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>323</v>
       </c>
@@ -7709,7 +7712,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>325</v>
       </c>
@@ -7741,7 +7744,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>326</v>
       </c>
@@ -7776,7 +7779,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>327</v>
       </c>
@@ -7846,7 +7849,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>329</v>
       </c>
@@ -7881,7 +7884,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>330</v>
       </c>
@@ -7916,7 +7919,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>331</v>
       </c>
@@ -7951,7 +7954,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>332</v>
       </c>
@@ -7986,7 +7989,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>333</v>
       </c>
@@ -8021,7 +8024,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>335</v>
       </c>
@@ -8056,7 +8059,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="183" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>337</v>
       </c>
@@ -8126,7 +8129,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>339</v>
       </c>
@@ -8161,7 +8164,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>340</v>
       </c>
@@ -8193,7 +8196,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>343</v>
       </c>
@@ -8228,7 +8231,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>345</v>
       </c>
@@ -8263,7 +8266,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>346</v>
       </c>
@@ -8298,7 +8301,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>348</v>
       </c>
@@ -8333,7 +8336,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>349</v>
       </c>
@@ -8368,7 +8371,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>350</v>
       </c>
@@ -8403,7 +8406,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>351</v>
       </c>
@@ -8438,7 +8441,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>352</v>
       </c>
@@ -8473,7 +8476,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>353</v>
       </c>
@@ -8543,7 +8546,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>355</v>
       </c>
@@ -8569,7 +8572,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="198" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>356</v>
       </c>
@@ -8604,7 +8607,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="199" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>357</v>
       </c>
@@ -8639,7 +8642,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>358</v>
       </c>
@@ -8674,7 +8677,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>359</v>
       </c>
@@ -8709,7 +8712,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>360</v>
       </c>
@@ -8744,7 +8747,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>361</v>
       </c>
@@ -8779,7 +8782,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>362</v>
       </c>
@@ -8814,7 +8817,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>364</v>
       </c>
@@ -8849,7 +8852,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>365</v>
       </c>
@@ -8884,7 +8887,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="207" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>366</v>
       </c>
@@ -8919,7 +8922,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>367</v>
       </c>
@@ -8954,7 +8957,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>368</v>
       </c>
@@ -8989,7 +8992,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>370</v>
       </c>
@@ -9024,7 +9027,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>371</v>
       </c>
@@ -9059,7 +9062,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>372</v>
       </c>
@@ -9094,7 +9097,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>373</v>
       </c>
@@ -9129,7 +9132,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>375</v>
       </c>
@@ -9164,7 +9167,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>376</v>
       </c>
@@ -9199,7 +9202,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>377</v>
       </c>
@@ -9234,7 +9237,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>378</v>
       </c>
@@ -9269,7 +9272,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="218" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>379</v>
       </c>
@@ -9304,7 +9307,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>380</v>
       </c>
@@ -9339,7 +9342,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>381</v>
       </c>
@@ -9374,7 +9377,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="221" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>382</v>
       </c>
@@ -9409,7 +9412,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>383</v>
       </c>
@@ -9444,7 +9447,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>384</v>
       </c>
@@ -9514,7 +9517,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>386</v>
       </c>
@@ -9549,7 +9552,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>387</v>
       </c>
@@ -9584,7 +9587,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>388</v>
       </c>
@@ -9619,7 +9622,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>389</v>
       </c>
@@ -9654,7 +9657,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="229" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>390</v>
       </c>
@@ -9689,7 +9692,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="230" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>391</v>
       </c>
@@ -9724,7 +9727,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="231" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>393</v>
       </c>
@@ -9759,7 +9762,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>394</v>
       </c>
@@ -9794,7 +9797,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="233" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>395</v>
       </c>
@@ -9829,7 +9832,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>396</v>
       </c>
@@ -9864,7 +9867,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>398</v>
       </c>
@@ -9899,7 +9902,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="236" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>399</v>
       </c>
@@ -9934,7 +9937,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>401</v>
       </c>
@@ -9969,7 +9972,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="238" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>402</v>
       </c>
@@ -10004,7 +10007,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>403</v>
       </c>
@@ -10039,7 +10042,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>404</v>
       </c>
@@ -10074,7 +10077,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>406</v>
       </c>
@@ -10109,7 +10112,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>407</v>
       </c>
@@ -10144,7 +10147,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>409</v>
       </c>
@@ -10179,7 +10182,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>410</v>
       </c>
@@ -10214,7 +10217,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="245" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>411</v>
       </c>
@@ -10249,7 +10252,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>412</v>
       </c>
@@ -10284,7 +10287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>414</v>
       </c>
@@ -10319,7 +10322,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>415</v>
       </c>
@@ -10354,7 +10357,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>416</v>
       </c>
@@ -10389,7 +10392,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>417</v>
       </c>
@@ -10424,7 +10427,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>419</v>
       </c>
@@ -10459,7 +10462,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>420</v>
       </c>
@@ -10494,7 +10497,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="253" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>421</v>
       </c>
@@ -10529,7 +10532,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>422</v>
       </c>
@@ -10561,7 +10564,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>424</v>
       </c>
@@ -10596,7 +10599,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>425</v>
       </c>
@@ -10631,7 +10634,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>426</v>
       </c>
@@ -10666,7 +10669,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="258" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>427</v>
       </c>
@@ -10701,7 +10704,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="259" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>429</v>
       </c>
@@ -10736,7 +10739,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="260" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>430</v>
       </c>
@@ -10771,7 +10774,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="261" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>431</v>
       </c>
@@ -10806,7 +10809,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="262" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>432</v>
       </c>
@@ -10841,7 +10844,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="263" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>434</v>
       </c>
@@ -10876,7 +10879,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>435</v>
       </c>
@@ -10911,7 +10914,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="265" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>436</v>
       </c>
@@ -10946,7 +10949,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>437</v>
       </c>
@@ -10981,7 +10984,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>439</v>
       </c>
@@ -11016,7 +11019,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>440</v>
       </c>
@@ -11051,7 +11054,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="269" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>441</v>
       </c>
@@ -11086,7 +11089,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>442</v>
       </c>
@@ -11121,7 +11124,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>444</v>
       </c>
@@ -11156,7 +11159,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>445</v>
       </c>
@@ -11191,7 +11194,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>446</v>
       </c>
@@ -11226,7 +11229,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>448</v>
       </c>
@@ -11261,7 +11264,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>449</v>
       </c>
@@ -11296,7 +11299,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>450</v>
       </c>
@@ -11331,7 +11334,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>451</v>
       </c>
@@ -11366,7 +11369,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>452</v>
       </c>
@@ -11401,7 +11404,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>453</v>
       </c>
@@ -11436,7 +11439,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>454</v>
       </c>
@@ -11506,7 +11509,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>457</v>
       </c>
@@ -11541,7 +11544,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>459</v>
       </c>
@@ -11576,7 +11579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>460</v>
       </c>
@@ -11611,7 +11614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>461</v>
       </c>
@@ -11646,7 +11649,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="286" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>462</v>
       </c>
@@ -11681,7 +11684,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>463</v>
       </c>
@@ -11716,7 +11719,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>465</v>
       </c>
@@ -11751,7 +11754,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="289" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>466</v>
       </c>
@@ -11786,7 +11789,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="290" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>468</v>
       </c>
@@ -11821,7 +11824,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="291" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>469</v>
       </c>
@@ -11856,7 +11859,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="292" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>470</v>
       </c>
@@ -11891,7 +11894,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="293" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>471</v>
       </c>
@@ -11926,7 +11929,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="294" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>472</v>
       </c>
@@ -11961,7 +11964,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="295" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>474</v>
       </c>
@@ -11996,7 +11999,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="296" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>475</v>
       </c>
@@ -12031,7 +12034,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="297" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>476</v>
       </c>

</xml_diff>